<commit_message>
mejoras en la lógica para lectura de facturas y agragada tabla para usd
</commit_message>
<xml_diff>
--- a/uploads/resultado.xlsx
+++ b/uploads/resultado.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,7 +441,12 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Importe</t>
+          <t>Importe_ARS</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Importe_USD</t>
         </is>
       </c>
     </row>
@@ -451,8 +456,15 @@
           <t>Fact 12334</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>45666</v>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>45.666,00</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>0,00</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -461,8 +473,15 @@
           <t>SIN FACTURA</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>98777</v>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>98.777,00</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>0,00</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -471,8 +490,15 @@
           <t>TOTAL GENERAL</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>144443</v>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>144.443,00</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>0,00</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>